<commit_message>
abiy - added wind profile inputs in the file
</commit_message>
<xml_diff>
--- a/modules/createEVENT/EmptyDomainCFD/sampleInputWindProfile.xlsx
+++ b/modules/createEVENT/EmptyDomainCFD/sampleInputWindProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanta\SimCenter\SourceCode\NHERI-SimCenter\SimCenterBackendApplications\modules\createEVENT\EmptyDomainCFD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\abiy\SimCenter\SourceCode\NHERI-SimCenter\SimCenterBackendApplications\modules\createEVENT\EmptyDomainCFD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9201428-C701-4A4D-BB44-15DDC5AD376C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B941F14-002E-49A6-96D0-8EED8A8BAE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{C4B59EDF-C0F3-4A3A-B325-CED103921929}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{C4B59EDF-C0F3-4A3A-B325-CED103921929}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,24 +50,6 @@
     <t>U</t>
   </si>
   <si>
-    <t>Ruu</t>
-  </si>
-  <si>
-    <t>Rvu</t>
-  </si>
-  <si>
-    <t>Rvv</t>
-  </si>
-  <si>
-    <t>Rwu</t>
-  </si>
-  <si>
-    <t>Rwv</t>
-  </si>
-  <si>
-    <t>Rww</t>
-  </si>
-  <si>
     <t>xLu</t>
   </si>
   <si>
@@ -94,11 +76,29 @@
   <si>
     <t>zLw</t>
   </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R22</t>
+  </si>
+  <si>
+    <t>R23</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -145,7 +145,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{89D1EBE6-5216-4D97-9F95-BEAA5AFD575A}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -158,9 +160,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -198,7 +200,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -304,7 +306,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,7 +448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,7 +459,7 @@
   <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -476,49 +478,49 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.45">

</xml_diff>